<commit_message>
Add domestic water processing.
</commit_message>
<xml_diff>
--- a/rgcam-data-system/rgcam-data/Mappings/UCS_tech_names.xlsx
+++ b/rgcam-data-system/rgcam-data/Mappings/UCS_tech_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19380" yWindow="2055" windowWidth="25125" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="5560" yWindow="0" windowWidth="23200" windowHeight="23300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="future" sheetId="1" r:id="rId1"/>
     <sheet name="base" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -837,16 +837,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -854,7 +854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -862,7 +862,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -870,7 +870,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -878,7 +878,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -886,7 +886,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -894,7 +894,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -902,7 +902,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -910,7 +910,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -918,7 +918,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -926,7 +926,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -934,7 +934,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -942,7 +942,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -950,7 +950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -958,7 +958,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -966,7 +966,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -974,7 +974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -982,7 +982,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -990,7 +990,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -998,7 +998,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1222,15 +1222,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1367,12 +1367,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>19</v>
       </c>

</xml_diff>